<commit_message>
Fix occupancy and checkout dashboard
</commit_message>
<xml_diff>
--- a/app/templates/report/occupancy.xlsx
+++ b/app/templates/report/occupancy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCE1680-3A9E-4502-9419-4D12A8F8BDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B07A2-DFAA-4C58-8812-EDC0CF9C81E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t xml:space="preserve">AVAILABLE BEDS </t>
   </si>
@@ -130,12 +130,6 @@
   </si>
   <si>
     <t>Building</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Location</t>
   </si>
   <si>
     <t>Resource</t>
@@ -455,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,9 +588,6 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1343,7 +1334,7 @@
   <sheetPr>
     <tabColor rgb="FF08BDBD"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1377,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="19">
-        <f>B5+B34</f>
+        <f>B5+B30</f>
         <v>0</v>
       </c>
     </row>
@@ -1386,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="20">
-        <f>B6+B18+B25+B29</f>
+        <f>B6+B17+B27+B23</f>
         <v>0</v>
       </c>
     </row>
@@ -1395,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="21">
-        <f>SUM(B7:B17)</f>
+        <f>SUM(B7:B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -1410,7 +1401,7 @@
     </row>
     <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="23">
         <f>IF($A8&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A8,'data-beds'!C:C),"")</f>
@@ -1455,7 +1446,7 @@
     </row>
     <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="23">
         <f>IF($A13&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A13,'data-beds'!C:C),"")</f>
@@ -1464,7 +1455,7 @@
     </row>
     <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="23">
         <f>IF($A14&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A14,'data-beds'!C:C),"")</f>
@@ -1473,7 +1464,7 @@
     </row>
     <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="23">
         <f>IF($A15&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A15,'data-beds'!C:C),"")</f>
@@ -1481,40 +1472,42 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="23" t="str">
+      <c r="A16" s="15"/>
+      <c r="B16" s="24" t="str">
         <f>IF($A16&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A16,'data-beds'!C:C),"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="24" t="str">
-        <f>IF($A17&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A17,'data-beds'!C:C),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="21">
-        <f>SUM(B19:B24)</f>
+      <c r="B17" s="21">
+        <f>SUM(B18:B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="22">
+        <f>IF($A18&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A18,'data-beds'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="22">
+      <c r="A19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="23">
         <f>IF($A19&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A19,'data-beds'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B20" s="23">
         <f>IF($A20&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A20,'data-beds'!C:C),"")</f>
@@ -1523,7 +1516,7 @@
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B21" s="23">
         <f>IF($A21&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A21,'data-beds'!C:C),"")</f>
@@ -1531,131 +1524,137 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="23" t="str">
+        <f>IF($A22&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A22,'data-beds'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="21">
+        <f>SUM(B24:B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="22">
+        <f>IF($A24&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A24,'data-beds'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="23">
+        <f>IF($A25&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A25,'data-beds'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="23" t="str">
+        <f>IF($A26&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A26,'data-beds'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="21">
+        <f>SUM(B28:B29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="22">
+        <f>IF($A28&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A28,'data-beds'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="23" t="str">
+        <f>IF($A29&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A29,'data-beds'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="20">
+        <f>SUM(B32:B43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="21">
+        <f t="shared" ref="B31" si="1">SUM(B32:B39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="22">
+        <f>IF($A32&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A32,'data-beds'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="23">
+        <f>IF($A33&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A33,'data-beds'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="23">
+        <f>IF($A34&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A34,'data-beds'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="23">
-        <f>IF($A22&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A22,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="23" t="str">
-        <f>IF($A23&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A23,'data-beds'!C:C),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="23" t="str">
-        <f>IF($A24&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A24,'data-beds'!C:C),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="21">
-        <f>SUM(B26:B28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="22">
-        <f>IF($A26&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A26,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="23" t="str">
-        <f>IF($A27&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A27,'data-beds'!C:C),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="23" t="str">
-        <f>IF($A28&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A28,'data-beds'!C:C),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="21">
-        <f>SUM(B30:B33)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="B35" s="23">
+        <f>IF($A35&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A35,'data-beds'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="22">
-        <f>IF($A30&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A30,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="23">
-        <f>IF($A31&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A31,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="23" t="str">
-        <f>IF($A32&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A32,'data-beds'!C:C),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="23" t="str">
-        <f>IF($A33&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A33,'data-beds'!C:C),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="20">
-        <f t="shared" ref="B34" si="1">SUM(B36:B48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="21">
-        <f t="shared" ref="B35" si="2">SUM(B36:B43)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="22">
+      <c r="B36" s="23">
         <f>IF($A36&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A36,'data-beds'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B37" s="23">
         <f>IF($A37&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A37,'data-beds'!C:C),"")</f>
@@ -1664,7 +1663,7 @@
     </row>
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B38" s="23">
         <f>IF($A38&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A38,'data-beds'!C:C),"")</f>
@@ -1682,7 +1681,7 @@
     </row>
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B40" s="23">
         <f>IF($A40&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A40,'data-beds'!C:C),"")</f>
@@ -1691,7 +1690,7 @@
     </row>
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B41" s="23">
         <f>IF($A41&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A41,'data-beds'!C:C),"")</f>
@@ -1700,7 +1699,7 @@
     </row>
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B42" s="23">
         <f>IF($A42&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A42,'data-beds'!C:C),"")</f>
@@ -1708,49 +1707,9 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="23">
+      <c r="A43" s="16"/>
+      <c r="B43" s="24" t="str">
         <f>IF($A43&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A43,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="23">
-        <f>IF($A44&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A44,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="23">
-        <f>IF($A45&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A45,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="23">
-        <f>IF($A46&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A46,'data-beds'!C:C),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="47"/>
-    </row>
-    <row r="48" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="24" t="str">
-        <f>IF($A48&lt;&gt;"",SUMIF('data-beds'!$A:$A,Beds!$A48,'data-beds'!C:C),"")</f>
         <v/>
       </c>
     </row>
@@ -1763,28 +1722,25 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:BP1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="2" width="21" customWidth="1"/>
+    <col min="3" max="68" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
@@ -1799,8 +1755,50 @@
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BE1" s="10"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="10"/>
+      <c r="BJ1" s="10"/>
+      <c r="BK1" s="10"/>
+      <c r="BL1" s="10"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="10"/>
+      <c r="BO1" s="10"/>
+      <c r="BP1" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1809,28 +1807,25 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:BP1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="2" width="21" customWidth="1"/>
+    <col min="3" max="68" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
@@ -1845,8 +1840,50 @@
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BE1" s="10"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="10"/>
+      <c r="BJ1" s="10"/>
+      <c r="BK1" s="10"/>
+      <c r="BL1" s="10"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="10"/>
+      <c r="BO1" s="10"/>
+      <c r="BP1" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1858,7 +1895,7 @@
   <sheetPr>
     <tabColor rgb="FF08BDBD"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -2008,41 +2045,41 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="15" t="str">
         <f>IF(Beds!A16&lt;&gt;"",Beds!A16,"")</f>
         <v/>
       </c>
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="38" t="str">
         <f>IF($A16&lt;&gt;"",IF(Beds!B16&lt;&gt;0,Nights!B16/(Occupancy!B$3*Beds!B16),0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="str">
         <f>IF(Beds!A17&lt;&gt;"",Beds!A17,"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="38" t="str">
+        <v>VALENCIA</v>
+      </c>
+      <c r="B17" s="34">
         <f>IF($A17&lt;&gt;"",IF(Beds!B17&lt;&gt;0,Nights!B17/(Occupancy!B$3*Beds!B17),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
         <f>IF(Beds!A18&lt;&gt;"",Beds!A18,"")</f>
-        <v>VALENCIA</v>
-      </c>
-      <c r="B18" s="34">
+        <v>Rodriguez De Cepeda 044</v>
+      </c>
+      <c r="B18" s="35">
         <f>IF($A18&lt;&gt;"",IF(Beds!B18&lt;&gt;0,Nights!B18/(Occupancy!B$3*Beds!B18),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="str">
+      <c r="A19" s="13" t="str">
         <f>IF(Beds!A19&lt;&gt;"",Beds!A19,"")</f>
-        <v>Rodriguez De Cepeda 044</v>
-      </c>
-      <c r="B19" s="35">
+        <v>Salamanca 46</v>
+      </c>
+      <c r="B19" s="36">
         <f>IF($A19&lt;&gt;"",IF(Beds!B19&lt;&gt;0,Nights!B19/(Occupancy!B$3*Beds!B19),0),"")</f>
         <v>0</v>
       </c>
@@ -2050,7 +2087,7 @@
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="str">
         <f>IF(Beds!A20&lt;&gt;"",Beds!A20,"")</f>
-        <v>Salamanca 46</v>
+        <v>Nau 14</v>
       </c>
       <c r="B20" s="36">
         <f>IF($A20&lt;&gt;"",IF(Beds!B20&lt;&gt;0,Nights!B20/(Occupancy!B$3*Beds!B20),0),"")</f>
@@ -2060,7 +2097,7 @@
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="str">
         <f>IF(Beds!A21&lt;&gt;"",Beds!A21,"")</f>
-        <v>Nau 14</v>
+        <v>Facultades</v>
       </c>
       <c r="B21" s="36">
         <f>IF($A21&lt;&gt;"",IF(Beds!B21&lt;&gt;0,Nights!B21/(Occupancy!B$3*Beds!B21),0),"")</f>
@@ -2068,151 +2105,151 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="15" t="str">
         <f>IF(Beds!A22&lt;&gt;"",Beds!A22,"")</f>
-        <v>Facultades</v>
-      </c>
-      <c r="B22" s="36">
+        <v/>
+      </c>
+      <c r="B22" s="38" t="str">
         <f>IF($A22&lt;&gt;"",IF(Beds!B22&lt;&gt;0,Nights!B22/(Occupancy!B$3*Beds!B22),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="str">
         <f>IF(Beds!A23&lt;&gt;"",Beds!A23,"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="36" t="str">
+        <v>MADRID</v>
+      </c>
+      <c r="B23" s="34">
         <f>IF($A23&lt;&gt;"",IF(Beds!B23&lt;&gt;0,Nights!B23/(Occupancy!B$3*Beds!B23),0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="str">
+      <c r="A24" s="12" t="str">
         <f>IF(Beds!A24&lt;&gt;"",Beds!A24,"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="38" t="str">
+        <v>Carlos III Campus Getafe</v>
+      </c>
+      <c r="B24" s="35">
         <f>IF($A24&lt;&gt;"",IF(Beds!B24&lt;&gt;0,Nights!B24/(Occupancy!B$3*Beds!B24),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
         <f>IF(Beds!A25&lt;&gt;"",Beds!A25,"")</f>
+        <v>Donoso Cortés 75</v>
+      </c>
+      <c r="B25" s="36">
+        <f>IF($A25&lt;&gt;"",IF(Beds!B25&lt;&gt;0,Nights!B25/(Occupancy!B$3*Beds!B25),0),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="str">
+        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+        <v/>
+      </c>
+      <c r="B26" s="38" t="str">
+        <f>IF($A26&lt;&gt;"",IF(Beds!B26&lt;&gt;0,Nights!B26/(Occupancy!B$3*Beds!B26),0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="str">
+        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
         <v>BILBAO</v>
       </c>
-      <c r="B25" s="34">
-        <f>IF($A25&lt;&gt;"",IF(Beds!B25&lt;&gt;0,Nights!B25/(Occupancy!B$3*Beds!B25),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
-        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+      <c r="B27" s="34">
+        <f>IF($A27&lt;&gt;"",IF(Beds!B27&lt;&gt;0,Nights!B27/(Occupancy!B$3*Beds!B27),0),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="str">
+        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
         <v>General Concha 24</v>
       </c>
-      <c r="B26" s="35">
-        <f>IF($A26&lt;&gt;"",IF(Beds!B26&lt;&gt;0,Nights!B26/(Occupancy!B$3*Beds!B26),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
-        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
-        <v/>
-      </c>
-      <c r="B27" s="36" t="str">
-        <f>IF($A27&lt;&gt;"",IF(Beds!B27&lt;&gt;0,Nights!B27/(Occupancy!B$3*Beds!B27),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="str">
-        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
-        <v/>
-      </c>
-      <c r="B28" s="38" t="str">
+      <c r="B28" s="35">
         <f>IF($A28&lt;&gt;"",IF(Beds!B28&lt;&gt;0,Nights!B28/(Occupancy!B$3*Beds!B28),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="str">
         <f>IF(Beds!A29&lt;&gt;"",Beds!A29,"")</f>
-        <v>MADRID</v>
-      </c>
-      <c r="B29" s="34">
+        <v/>
+      </c>
+      <c r="B29" s="38" t="str">
         <f>IF($A29&lt;&gt;"",IF(Beds!B29&lt;&gt;0,Nights!B29/(Occupancy!B$3*Beds!B29),0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="str">
+      <c r="A30" s="4" t="str">
         <f>IF(Beds!A30&lt;&gt;"",Beds!A30,"")</f>
-        <v>Carlos III Campus Getafe</v>
-      </c>
-      <c r="B30" s="35">
+        <v>3rd PARTIES</v>
+      </c>
+      <c r="B30" s="33">
         <f>IF($A30&lt;&gt;"",IF(Beds!B30&lt;&gt;0,Nights!B30/(Occupancy!B$3*Beds!B30),0),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="str">
         <f>IF(Beds!A31&lt;&gt;"",Beds!A31,"")</f>
-        <v>Donoso Cortés 75</v>
-      </c>
-      <c r="B31" s="36">
+        <v>BARCELONA</v>
+      </c>
+      <c r="B31" s="34">
         <f>IF($A31&lt;&gt;"",IF(Beds!B31&lt;&gt;0,Nights!B31/(Occupancy!B$3*Beds!B31),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="12" t="str">
         <f>IF(Beds!A32&lt;&gt;"",Beds!A32,"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="36" t="str">
+        <v>Artesania 30</v>
+      </c>
+      <c r="B32" s="35">
         <f>IF($A32&lt;&gt;"",IF(Beds!B32&lt;&gt;0,Nights!B32/(Occupancy!B$3*Beds!B32),0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="str">
+      <c r="A33" s="13" t="str">
         <f>IF(Beds!A33&lt;&gt;"",Beds!A33,"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="38" t="str">
+        <v>Bailén 33</v>
+      </c>
+      <c r="B33" s="36">
         <f>IF($A33&lt;&gt;"",IF(Beds!B33&lt;&gt;0,Nights!B33/(Occupancy!B$3*Beds!B33),0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="str">
+      <c r="A34" s="13" t="str">
         <f>IF(Beds!A34&lt;&gt;"",Beds!A34,"")</f>
-        <v>3rd PARTIES</v>
-      </c>
-      <c r="B34" s="33">
+        <v>Consell De Cent 222</v>
+      </c>
+      <c r="B34" s="36">
         <f>IF($A34&lt;&gt;"",IF(Beds!B34&lt;&gt;0,Nights!B34/(Occupancy!B$3*Beds!B34),0),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="str">
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="str">
         <f>IF(Beds!A35&lt;&gt;"",Beds!A35,"")</f>
-        <v>BARCELONA</v>
-      </c>
-      <c r="B35" s="34">
+        <v>Còrsega 52</v>
+      </c>
+      <c r="B35" s="36">
         <f>IF($A35&lt;&gt;"",IF(Beds!B35&lt;&gt;0,Nights!B35/(Occupancy!B$3*Beds!B35),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="str">
+      <c r="A36" s="13" t="str">
         <f>IF(Beds!A36&lt;&gt;"",Beds!A36,"")</f>
-        <v>Artesania 30</v>
-      </c>
-      <c r="B36" s="35">
+        <v>Còrsega 207</v>
+      </c>
+      <c r="B36" s="36">
         <f>IF($A36&lt;&gt;"",IF(Beds!B36&lt;&gt;0,Nights!B36/(Occupancy!B$3*Beds!B36),0),"")</f>
         <v>0</v>
       </c>
@@ -2220,7 +2257,7 @@
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f>IF(Beds!A37&lt;&gt;"",Beds!A37,"")</f>
-        <v>Bailén 33</v>
+        <v>Encarnación 160</v>
       </c>
       <c r="B37" s="36">
         <f>IF($A37&lt;&gt;"",IF(Beds!B37&lt;&gt;0,Nights!B37/(Occupancy!B$3*Beds!B37),0),"")</f>
@@ -2230,7 +2267,7 @@
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f>IF(Beds!A38&lt;&gt;"",Beds!A38,"")</f>
-        <v>Consell De Cent 222</v>
+        <v>Gran Via 598</v>
       </c>
       <c r="B38" s="36">
         <f>IF($A38&lt;&gt;"",IF(Beds!B38&lt;&gt;0,Nights!B38/(Occupancy!B$3*Beds!B38),0),"")</f>
@@ -2240,7 +2277,7 @@
     <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f>IF(Beds!A39&lt;&gt;"",Beds!A39,"")</f>
-        <v>Còrsega 52</v>
+        <v>Ramón Albó 6</v>
       </c>
       <c r="B39" s="36">
         <f>IF($A39&lt;&gt;"",IF(Beds!B39&lt;&gt;0,Nights!B39/(Occupancy!B$3*Beds!B39),0),"")</f>
@@ -2250,7 +2287,7 @@
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f>IF(Beds!A40&lt;&gt;"",Beds!A40,"")</f>
-        <v>Còrsega 207</v>
+        <v>Robrenyo 67</v>
       </c>
       <c r="B40" s="36">
         <f>IF($A40&lt;&gt;"",IF(Beds!B40&lt;&gt;0,Nights!B40/(Occupancy!B$3*Beds!B40),0),"")</f>
@@ -2260,7 +2297,7 @@
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f>IF(Beds!A41&lt;&gt;"",Beds!A41,"")</f>
-        <v>Encarnación 160</v>
+        <v>Sardenya 326</v>
       </c>
       <c r="B41" s="36">
         <f>IF($A41&lt;&gt;"",IF(Beds!B41&lt;&gt;0,Nights!B41/(Occupancy!B$3*Beds!B41),0),"")</f>
@@ -2270,7 +2307,7 @@
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f>IF(Beds!A42&lt;&gt;"",Beds!A42,"")</f>
-        <v>Gran Via 598</v>
+        <v>Travessera 43</v>
       </c>
       <c r="B42" s="36">
         <f>IF($A42&lt;&gt;"",IF(Beds!B42&lt;&gt;0,Nights!B42/(Occupancy!B$3*Beds!B42),0),"")</f>
@@ -2278,56 +2315,12 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="str">
+      <c r="A43" s="16" t="str">
         <f>IF(Beds!A43&lt;&gt;"",Beds!A43,"")</f>
-        <v>Ramón Albó 6</v>
-      </c>
-      <c r="B43" s="36">
+        <v/>
+      </c>
+      <c r="B43" s="38" t="str">
         <f>IF($A43&lt;&gt;"",IF(Beds!B43&lt;&gt;0,Nights!B43/(Occupancy!B$3*Beds!B43),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="str">
-        <f>IF(Beds!A44&lt;&gt;"",Beds!A44,"")</f>
-        <v>Robrenyo 67</v>
-      </c>
-      <c r="B44" s="36">
-        <f>IF($A44&lt;&gt;"",IF(Beds!B44&lt;&gt;0,Nights!B44/(Occupancy!B$3*Beds!B44),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="str">
-        <f>IF(Beds!A45&lt;&gt;"",Beds!A45,"")</f>
-        <v>Sardenya 326</v>
-      </c>
-      <c r="B45" s="36">
-        <f>IF($A45&lt;&gt;"",IF(Beds!B45&lt;&gt;0,Nights!B45/(Occupancy!B$3*Beds!B45),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="str">
-        <f>IF(Beds!A46&lt;&gt;"",Beds!A46,"")</f>
-        <v>Travessera 43</v>
-      </c>
-      <c r="B46" s="36">
-        <f>IF($A46&lt;&gt;"",IF(Beds!B46&lt;&gt;0,Nights!B46/(Occupancy!B$3*Beds!B46),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="37"/>
-    </row>
-    <row r="48" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="str">
-        <f>IF(Beds!A48&lt;&gt;"",Beds!A48,"")</f>
-        <v/>
-      </c>
-      <c r="B48" s="38" t="str">
-        <f>IF($A48&lt;&gt;"",IF(Beds!B48&lt;&gt;0,Nights!B48/(Occupancy!B$3*Beds!B48),0),"")</f>
         <v/>
       </c>
     </row>
@@ -2343,7 +2336,7 @@
   <sheetPr>
     <tabColor rgb="FF08BDBD"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -2358,7 +2351,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="17">
         <f>'data-beds'!C1</f>
@@ -2378,7 +2371,7 @@
         <v>TOTAL</v>
       </c>
       <c r="B4" s="25">
-        <f>B5+B34</f>
+        <f>B5+B30</f>
         <v>0</v>
       </c>
     </row>
@@ -2388,7 +2381,7 @@
         <v>VANDOR</v>
       </c>
       <c r="B5" s="26">
-        <f>B6+B18+B25+B29</f>
+        <f>B6+B17+B27+B23</f>
         <v>0</v>
       </c>
     </row>
@@ -2398,7 +2391,7 @@
         <v>BARCELONA</v>
       </c>
       <c r="B6" s="27">
-        <f>SUM(B7:B17)</f>
+        <f>SUM(B7:B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -2408,7 +2401,7 @@
         <v>Balmes 335</v>
       </c>
       <c r="B7" s="28">
-        <f>IF($A7&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A7,'data-rent'!E:E),"")</f>
+        <f>IF($A7&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A7,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2418,7 +2411,7 @@
         <v>Nàpols 206</v>
       </c>
       <c r="B8" s="29">
-        <f>IF($A8&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A8,'data-rent'!E:E),"")</f>
+        <f>IF($A8&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A8,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2428,7 +2421,7 @@
         <v>Rocafort 219</v>
       </c>
       <c r="B9" s="29">
-        <f>IF($A9&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A9,'data-rent'!E:E),"")</f>
+        <f>IF($A9&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A9,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2438,7 +2431,7 @@
         <v>Entença 069</v>
       </c>
       <c r="B10" s="29">
-        <f>IF($A10&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A10,'data-rent'!E:E),"")</f>
+        <f>IF($A10&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A10,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2448,7 +2441,7 @@
         <v>Avenida Madrid 110</v>
       </c>
       <c r="B11" s="29">
-        <f>IF($A11&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A11,'data-rent'!E:E),"")</f>
+        <f>IF($A11&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A11,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2458,7 +2451,7 @@
         <v>Muntaner 448</v>
       </c>
       <c r="B12" s="29">
-        <f>IF($A12&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A12,'data-rent'!E:E),"")</f>
+        <f>IF($A12&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A12,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2468,7 +2461,7 @@
         <v>Concordia 12</v>
       </c>
       <c r="B13" s="29">
-        <f>IF($A13&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A13,'data-rent'!E:E),"")</f>
+        <f>IF($A13&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A13,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2478,7 +2471,7 @@
         <v>Consell De Cent 538</v>
       </c>
       <c r="B14" s="29">
-        <f>IF($A14&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A14,'data-rent'!E:E),"")</f>
+        <f>IF($A14&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A14,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2488,331 +2481,287 @@
         <v>Còrsega 396</v>
       </c>
       <c r="B15" s="30">
-        <f>IF($A15&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A15,'data-rent'!E:E),"")</f>
+        <f>IF($A15&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A15,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="15" t="str">
         <f>IF(Beds!A16&lt;&gt;"",Beds!A16,"")</f>
         <v/>
       </c>
-      <c r="B16" s="30" t="str">
-        <f>IF($A16&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A16,'data-rent'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+      <c r="B16" s="31" t="str">
+        <f>IF($A16&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A16,'data-rent'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="str">
         <f>IF(Beds!A17&lt;&gt;"",Beds!A17,"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="31" t="str">
-        <f>IF($A17&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A17,'data-rent'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
+        <v>VALENCIA</v>
+      </c>
+      <c r="B17" s="27">
+        <f>SUM(B18:B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
         <f>IF(Beds!A18&lt;&gt;"",Beds!A18,"")</f>
-        <v>VALENCIA</v>
-      </c>
-      <c r="B18" s="27">
-        <f>SUM(B19:B24)</f>
+        <v>Rodriguez De Cepeda 044</v>
+      </c>
+      <c r="B18" s="28">
+        <f>IF($A18&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A18,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="str">
+      <c r="A19" s="13" t="str">
         <f>IF(Beds!A19&lt;&gt;"",Beds!A19,"")</f>
-        <v>Rodriguez De Cepeda 044</v>
-      </c>
-      <c r="B19" s="28">
-        <f>IF($A19&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A19,'data-rent'!E:E),"")</f>
+        <v>Salamanca 46</v>
+      </c>
+      <c r="B19" s="29">
+        <f>IF($A19&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A19,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="str">
         <f>IF(Beds!A20&lt;&gt;"",Beds!A20,"")</f>
-        <v>Salamanca 46</v>
+        <v>Nau 14</v>
       </c>
       <c r="B20" s="29">
-        <f>IF($A20&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A20,'data-rent'!E:E),"")</f>
+        <f>IF($A20&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A20,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="str">
         <f>IF(Beds!A21&lt;&gt;"",Beds!A21,"")</f>
-        <v>Nau 14</v>
+        <v>Facultades</v>
       </c>
       <c r="B21" s="29">
-        <f>IF($A21&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A21,'data-rent'!E:E),"")</f>
+        <f>IF($A21&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A21,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="15" t="str">
         <f>IF(Beds!A22&lt;&gt;"",Beds!A22,"")</f>
-        <v>Facultades</v>
-      </c>
-      <c r="B22" s="29">
-        <f>IF($A22&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A22,'data-rent'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
+        <v/>
+      </c>
+      <c r="B22" s="31" t="str">
+        <f>IF($A22&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A22,'data-rent'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="str">
         <f>IF(Beds!A23&lt;&gt;"",Beds!A23,"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="29" t="str">
-        <f>IF($A23&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A23,'data-rent'!E:E),"")</f>
-        <v/>
+        <v>MADRID</v>
+      </c>
+      <c r="B23" s="27">
+        <f>SUM(B24:B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="str">
+      <c r="A24" s="12" t="str">
         <f>IF(Beds!A24&lt;&gt;"",Beds!A24,"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="31" t="str">
-        <f>IF($A24&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A24,'data-rent'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="str">
+        <v>Carlos III Campus Getafe</v>
+      </c>
+      <c r="B24" s="28">
+        <f>IF($A24&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A24,'data-rent'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
         <f>IF(Beds!A25&lt;&gt;"",Beds!A25,"")</f>
+        <v>Donoso Cortés 75</v>
+      </c>
+      <c r="B25" s="29">
+        <f>IF($A25&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A25,'data-rent'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="str">
+        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+        <v/>
+      </c>
+      <c r="B26" s="31" t="str">
+        <f>IF($A26&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A26,'data-rent'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="str">
+        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
         <v>BILBAO</v>
       </c>
-      <c r="B25" s="27">
-        <f>SUM(B26:B28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
-        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+      <c r="B27" s="27">
+        <f>SUM(B28:B29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="str">
+        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
         <v>General Concha 24</v>
       </c>
-      <c r="B26" s="28">
-        <f>IF($A26&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A26,'data-rent'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
-        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
-        <v/>
-      </c>
-      <c r="B27" s="29" t="str">
-        <f>IF($A27&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A27,'data-rent'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="str">
-        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
-        <v/>
-      </c>
-      <c r="B28" s="31" t="str">
-        <f>IF($A28&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A28,'data-rent'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="str">
+      <c r="B28" s="28">
+        <f>IF($A28&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A28,'data-rent'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="str">
         <f>IF(Beds!A29&lt;&gt;"",Beds!A29,"")</f>
-        <v>MADRID</v>
-      </c>
-      <c r="B29" s="27">
-        <f>SUM(B30:B33)</f>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="B29" s="31" t="str">
+        <f>IF($A29&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A29,'data-rent'!C:C),"")</f>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="str">
+      <c r="A30" s="4" t="str">
         <f>IF(Beds!A30&lt;&gt;"",Beds!A30,"")</f>
-        <v>Carlos III Campus Getafe</v>
-      </c>
-      <c r="B30" s="28">
-        <f>IF($A30&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A30,'data-rent'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+        <v>3rd PARTIES</v>
+      </c>
+      <c r="B30" s="26">
+        <f>SUM(B32:B43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="str">
         <f>IF(Beds!A31&lt;&gt;"",Beds!A31,"")</f>
-        <v>Donoso Cortés 75</v>
-      </c>
-      <c r="B31" s="29">
-        <f>IF($A31&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A31,'data-rent'!E:E),"")</f>
+        <v>BARCELONA</v>
+      </c>
+      <c r="B31" s="27">
+        <f t="shared" ref="B31" si="1">SUM(B32:B39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="12" t="str">
         <f>IF(Beds!A32&lt;&gt;"",Beds!A32,"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="29" t="str">
-        <f>IF($A32&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A32,'data-rent'!E:E),"")</f>
-        <v/>
+        <v>Artesania 30</v>
+      </c>
+      <c r="B32" s="28">
+        <f>IF($A32&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A32,'data-rent'!C:C),"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="str">
+      <c r="A33" s="13" t="str">
         <f>IF(Beds!A33&lt;&gt;"",Beds!A33,"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="31" t="str">
-        <f>IF($A33&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A33,'data-rent'!E:E),"")</f>
-        <v/>
+        <v>Bailén 33</v>
+      </c>
+      <c r="B33" s="29">
+        <f>IF($A33&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A33,'data-rent'!C:C),"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="str">
+      <c r="A34" s="13" t="str">
         <f>IF(Beds!A34&lt;&gt;"",Beds!A34,"")</f>
-        <v>3rd PARTIES</v>
-      </c>
-      <c r="B34" s="26">
-        <f t="shared" ref="B34" si="1">SUM(B36:B48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="str">
+        <v>Consell De Cent 222</v>
+      </c>
+      <c r="B34" s="29">
+        <f>IF($A34&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A34,'data-rent'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="str">
         <f>IF(Beds!A35&lt;&gt;"",Beds!A35,"")</f>
-        <v>BARCELONA</v>
-      </c>
-      <c r="B35" s="27">
-        <f t="shared" ref="B35" si="2">SUM(B36:B43)</f>
+        <v>Còrsega 52</v>
+      </c>
+      <c r="B35" s="29">
+        <f>IF($A35&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A35,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="str">
+      <c r="A36" s="13" t="str">
         <f>IF(Beds!A36&lt;&gt;"",Beds!A36,"")</f>
-        <v>Artesania 30</v>
-      </c>
-      <c r="B36" s="28">
-        <f>IF($A36&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A36,'data-rent'!E:E),"")</f>
+        <v>Còrsega 207</v>
+      </c>
+      <c r="B36" s="29">
+        <f>IF($A36&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A36,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f>IF(Beds!A37&lt;&gt;"",Beds!A37,"")</f>
-        <v>Bailén 33</v>
+        <v>Encarnación 160</v>
       </c>
       <c r="B37" s="29">
-        <f>IF($A37&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A37,'data-rent'!E:E),"")</f>
+        <f>IF($A37&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A37,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f>IF(Beds!A38&lt;&gt;"",Beds!A38,"")</f>
-        <v>Consell De Cent 222</v>
+        <v>Gran Via 598</v>
       </c>
       <c r="B38" s="29">
-        <f>IF($A38&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A38,'data-rent'!E:E),"")</f>
+        <f>IF($A38&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A38,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f>IF(Beds!A39&lt;&gt;"",Beds!A39,"")</f>
-        <v>Còrsega 52</v>
+        <v>Ramón Albó 6</v>
       </c>
       <c r="B39" s="29">
-        <f>IF($A39&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A39,'data-rent'!E:E),"")</f>
+        <f>IF($A39&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A39,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f>IF(Beds!A40&lt;&gt;"",Beds!A40,"")</f>
-        <v>Còrsega 207</v>
+        <v>Robrenyo 67</v>
       </c>
       <c r="B40" s="29">
-        <f>IF($A40&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A40,'data-rent'!E:E),"")</f>
+        <f>IF($A40&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A40,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f>IF(Beds!A41&lt;&gt;"",Beds!A41,"")</f>
-        <v>Encarnación 160</v>
+        <v>Sardenya 326</v>
       </c>
       <c r="B41" s="29">
-        <f>IF($A41&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A41,'data-rent'!E:E),"")</f>
+        <f>IF($A41&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A41,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f>IF(Beds!A42&lt;&gt;"",Beds!A42,"")</f>
-        <v>Gran Via 598</v>
+        <v>Travessera 43</v>
       </c>
       <c r="B42" s="29">
-        <f>IF($A42&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A42,'data-rent'!E:E),"")</f>
+        <f>IF($A42&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A42,'data-rent'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="str">
+      <c r="A43" s="16" t="str">
         <f>IF(Beds!A43&lt;&gt;"",Beds!A43,"")</f>
-        <v>Ramón Albó 6</v>
-      </c>
-      <c r="B43" s="29">
-        <f>IF($A43&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A43,'data-rent'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="str">
-        <f>IF(Beds!A44&lt;&gt;"",Beds!A44,"")</f>
-        <v>Robrenyo 67</v>
-      </c>
-      <c r="B44" s="29">
-        <f>IF($A44&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A44,'data-rent'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="str">
-        <f>IF(Beds!A45&lt;&gt;"",Beds!A45,"")</f>
-        <v>Sardenya 326</v>
-      </c>
-      <c r="B45" s="29">
-        <f>IF($A45&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A45,'data-rent'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="str">
-        <f>IF(Beds!A46&lt;&gt;"",Beds!A46,"")</f>
-        <v>Travessera 43</v>
-      </c>
-      <c r="B46" s="29">
-        <f>IF($A46&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A46,'data-rent'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="str">
-        <f>IF(Beds!A48&lt;&gt;"",Beds!A48,"")</f>
-        <v/>
-      </c>
-      <c r="B48" s="31" t="str">
-        <f>IF($A48&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A48,'data-rent'!E:E),"")</f>
+        <v/>
+      </c>
+      <c r="B43" s="31" t="str">
+        <f>IF($A43&lt;&gt;"",SUMIF('data-rent'!$A:$A,$A43,'data-rent'!C:C),"")</f>
         <v/>
       </c>
     </row>
@@ -2828,7 +2777,7 @@
   <sheetPr>
     <tabColor rgb="FF08BDBD"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -2843,7 +2792,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="17">
         <f>'data-beds'!C1</f>
@@ -2863,7 +2812,7 @@
         <v>TOTAL</v>
       </c>
       <c r="B4" s="25">
-        <f>B5+B34</f>
+        <f>B5+B30</f>
         <v>0</v>
       </c>
     </row>
@@ -2873,7 +2822,7 @@
         <v>VANDOR</v>
       </c>
       <c r="B5" s="26">
-        <f>B6+B18+B25+B29</f>
+        <f>B6+B17+B27+B23</f>
         <v>0</v>
       </c>
     </row>
@@ -2883,7 +2832,7 @@
         <v>BARCELONA</v>
       </c>
       <c r="B6" s="27">
-        <f>SUM(B7:B17)</f>
+        <f>SUM(B7:B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -2893,7 +2842,7 @@
         <v>Balmes 335</v>
       </c>
       <c r="B7" s="28">
-        <f>IF($A7&lt;&gt;"",SUMIF('data-services'!$A:$A,$A7,'data-services'!E:E),"")</f>
+        <f>IF($A7&lt;&gt;"",SUMIF('data-services'!$A:$A,$A7,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2903,7 +2852,7 @@
         <v>Nàpols 206</v>
       </c>
       <c r="B8" s="29">
-        <f>IF($A8&lt;&gt;"",SUMIF('data-services'!$A:$A,$A8,'data-services'!E:E),"")</f>
+        <f>IF($A8&lt;&gt;"",SUMIF('data-services'!$A:$A,$A8,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2913,7 +2862,7 @@
         <v>Rocafort 219</v>
       </c>
       <c r="B9" s="29">
-        <f>IF($A9&lt;&gt;"",SUMIF('data-services'!$A:$A,$A9,'data-services'!E:E),"")</f>
+        <f>IF($A9&lt;&gt;"",SUMIF('data-services'!$A:$A,$A9,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2923,7 +2872,7 @@
         <v>Entença 069</v>
       </c>
       <c r="B10" s="29">
-        <f>IF($A10&lt;&gt;"",SUMIF('data-services'!$A:$A,$A10,'data-services'!E:E),"")</f>
+        <f>IF($A10&lt;&gt;"",SUMIF('data-services'!$A:$A,$A10,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2933,7 +2882,7 @@
         <v>Avenida Madrid 110</v>
       </c>
       <c r="B11" s="29">
-        <f>IF($A11&lt;&gt;"",SUMIF('data-services'!$A:$A,$A11,'data-services'!E:E),"")</f>
+        <f>IF($A11&lt;&gt;"",SUMIF('data-services'!$A:$A,$A11,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2943,7 +2892,7 @@
         <v>Muntaner 448</v>
       </c>
       <c r="B12" s="29">
-        <f>IF($A12&lt;&gt;"",SUMIF('data-services'!$A:$A,$A12,'data-services'!E:E),"")</f>
+        <f>IF($A12&lt;&gt;"",SUMIF('data-services'!$A:$A,$A12,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2953,7 +2902,7 @@
         <v>Concordia 12</v>
       </c>
       <c r="B13" s="29">
-        <f>IF($A13&lt;&gt;"",SUMIF('data-services'!$A:$A,$A13,'data-services'!E:E),"")</f>
+        <f>IF($A13&lt;&gt;"",SUMIF('data-services'!$A:$A,$A13,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2963,7 +2912,7 @@
         <v>Consell De Cent 538</v>
       </c>
       <c r="B14" s="29">
-        <f>IF($A14&lt;&gt;"",SUMIF('data-services'!$A:$A,$A14,'data-services'!E:E),"")</f>
+        <f>IF($A14&lt;&gt;"",SUMIF('data-services'!$A:$A,$A14,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2973,331 +2922,287 @@
         <v>Còrsega 396</v>
       </c>
       <c r="B15" s="30">
-        <f>IF($A15&lt;&gt;"",SUMIF('data-services'!$A:$A,$A15,'data-services'!E:E),"")</f>
+        <f>IF($A15&lt;&gt;"",SUMIF('data-services'!$A:$A,$A15,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="15" t="str">
         <f>IF(Beds!A16&lt;&gt;"",Beds!A16,"")</f>
         <v/>
       </c>
-      <c r="B16" s="30" t="str">
-        <f>IF($A16&lt;&gt;"",SUMIF('data-services'!$A:$A,$A16,'data-services'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+      <c r="B16" s="31" t="str">
+        <f>IF($A16&lt;&gt;"",SUMIF('data-services'!$A:$A,$A16,'data-services'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="str">
         <f>IF(Beds!A17&lt;&gt;"",Beds!A17,"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="31" t="str">
-        <f>IF($A17&lt;&gt;"",SUMIF('data-services'!$A:$A,$A17,'data-services'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
+        <v>VALENCIA</v>
+      </c>
+      <c r="B17" s="27">
+        <f>SUM(B18:B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
         <f>IF(Beds!A18&lt;&gt;"",Beds!A18,"")</f>
-        <v>VALENCIA</v>
-      </c>
-      <c r="B18" s="27">
-        <f>SUM(B19:B24)</f>
+        <v>Rodriguez De Cepeda 044</v>
+      </c>
+      <c r="B18" s="28">
+        <f>IF($A18&lt;&gt;"",SUMIF('data-services'!$A:$A,$A18,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="str">
+      <c r="A19" s="13" t="str">
         <f>IF(Beds!A19&lt;&gt;"",Beds!A19,"")</f>
-        <v>Rodriguez De Cepeda 044</v>
-      </c>
-      <c r="B19" s="28">
-        <f>IF($A19&lt;&gt;"",SUMIF('data-services'!$A:$A,$A19,'data-services'!E:E),"")</f>
+        <v>Salamanca 46</v>
+      </c>
+      <c r="B19" s="29">
+        <f>IF($A19&lt;&gt;"",SUMIF('data-services'!$A:$A,$A19,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="str">
         <f>IF(Beds!A20&lt;&gt;"",Beds!A20,"")</f>
-        <v>Salamanca 46</v>
+        <v>Nau 14</v>
       </c>
       <c r="B20" s="29">
-        <f>IF($A20&lt;&gt;"",SUMIF('data-services'!$A:$A,$A20,'data-services'!E:E),"")</f>
+        <f>IF($A20&lt;&gt;"",SUMIF('data-services'!$A:$A,$A20,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="str">
         <f>IF(Beds!A21&lt;&gt;"",Beds!A21,"")</f>
-        <v>Nau 14</v>
+        <v>Facultades</v>
       </c>
       <c r="B21" s="29">
-        <f>IF($A21&lt;&gt;"",SUMIF('data-services'!$A:$A,$A21,'data-services'!E:E),"")</f>
+        <f>IF($A21&lt;&gt;"",SUMIF('data-services'!$A:$A,$A21,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="15" t="str">
         <f>IF(Beds!A22&lt;&gt;"",Beds!A22,"")</f>
-        <v>Facultades</v>
-      </c>
-      <c r="B22" s="29">
-        <f>IF($A22&lt;&gt;"",SUMIF('data-services'!$A:$A,$A22,'data-services'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
+        <v/>
+      </c>
+      <c r="B22" s="31" t="str">
+        <f>IF($A22&lt;&gt;"",SUMIF('data-services'!$A:$A,$A22,'data-services'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="str">
         <f>IF(Beds!A23&lt;&gt;"",Beds!A23,"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="29" t="str">
-        <f>IF($A23&lt;&gt;"",SUMIF('data-services'!$A:$A,$A23,'data-services'!E:E),"")</f>
-        <v/>
+        <v>MADRID</v>
+      </c>
+      <c r="B23" s="27">
+        <f>SUM(B24:B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="str">
+      <c r="A24" s="12" t="str">
         <f>IF(Beds!A24&lt;&gt;"",Beds!A24,"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="31" t="str">
-        <f>IF($A24&lt;&gt;"",SUMIF('data-services'!$A:$A,$A24,'data-services'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="str">
+        <v>Carlos III Campus Getafe</v>
+      </c>
+      <c r="B24" s="28">
+        <f>IF($A24&lt;&gt;"",SUMIF('data-services'!$A:$A,$A24,'data-services'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
         <f>IF(Beds!A25&lt;&gt;"",Beds!A25,"")</f>
+        <v>Donoso Cortés 75</v>
+      </c>
+      <c r="B25" s="29">
+        <f>IF($A25&lt;&gt;"",SUMIF('data-services'!$A:$A,$A25,'data-services'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="str">
+        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+        <v/>
+      </c>
+      <c r="B26" s="31" t="str">
+        <f>IF($A26&lt;&gt;"",SUMIF('data-services'!$A:$A,$A26,'data-services'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="str">
+        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
         <v>BILBAO</v>
       </c>
-      <c r="B25" s="27">
-        <f>SUM(B26:B28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
-        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+      <c r="B27" s="27">
+        <f>SUM(B28:B29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="str">
+        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
         <v>General Concha 24</v>
       </c>
-      <c r="B26" s="28">
-        <f>IF($A26&lt;&gt;"",SUMIF('data-services'!$A:$A,$A26,'data-services'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
-        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
-        <v/>
-      </c>
-      <c r="B27" s="29" t="str">
-        <f>IF($A27&lt;&gt;"",SUMIF('data-services'!$A:$A,$A27,'data-services'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="str">
-        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
-        <v/>
-      </c>
-      <c r="B28" s="31" t="str">
-        <f>IF($A28&lt;&gt;"",SUMIF('data-services'!$A:$A,$A28,'data-services'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="str">
+      <c r="B28" s="28">
+        <f>IF($A28&lt;&gt;"",SUMIF('data-services'!$A:$A,$A28,'data-services'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="str">
         <f>IF(Beds!A29&lt;&gt;"",Beds!A29,"")</f>
-        <v>MADRID</v>
-      </c>
-      <c r="B29" s="27">
-        <f>SUM(B30:B33)</f>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="B29" s="31" t="str">
+        <f>IF($A29&lt;&gt;"",SUMIF('data-services'!$A:$A,$A29,'data-services'!C:C),"")</f>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="str">
+      <c r="A30" s="4" t="str">
         <f>IF(Beds!A30&lt;&gt;"",Beds!A30,"")</f>
-        <v>Carlos III Campus Getafe</v>
-      </c>
-      <c r="B30" s="28">
-        <f>IF($A30&lt;&gt;"",SUMIF('data-services'!$A:$A,$A30,'data-services'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+        <v>3rd PARTIES</v>
+      </c>
+      <c r="B30" s="26">
+        <f>SUM(B32:B43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="str">
         <f>IF(Beds!A31&lt;&gt;"",Beds!A31,"")</f>
-        <v>Donoso Cortés 75</v>
-      </c>
-      <c r="B31" s="29">
-        <f>IF($A31&lt;&gt;"",SUMIF('data-services'!$A:$A,$A31,'data-services'!E:E),"")</f>
+        <v>BARCELONA</v>
+      </c>
+      <c r="B31" s="27">
+        <f t="shared" ref="B31" si="1">SUM(B32:B39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="12" t="str">
         <f>IF(Beds!A32&lt;&gt;"",Beds!A32,"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="29" t="str">
-        <f>IF($A32&lt;&gt;"",SUMIF('data-services'!$A:$A,$A32,'data-services'!E:E),"")</f>
-        <v/>
+        <v>Artesania 30</v>
+      </c>
+      <c r="B32" s="28">
+        <f>IF($A32&lt;&gt;"",SUMIF('data-services'!$A:$A,$A32,'data-services'!C:C),"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="str">
+      <c r="A33" s="13" t="str">
         <f>IF(Beds!A33&lt;&gt;"",Beds!A33,"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="31" t="str">
-        <f>IF($A33&lt;&gt;"",SUMIF('data-services'!$A:$A,$A33,'data-services'!E:E),"")</f>
-        <v/>
+        <v>Bailén 33</v>
+      </c>
+      <c r="B33" s="29">
+        <f>IF($A33&lt;&gt;"",SUMIF('data-services'!$A:$A,$A33,'data-services'!C:C),"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="str">
+      <c r="A34" s="13" t="str">
         <f>IF(Beds!A34&lt;&gt;"",Beds!A34,"")</f>
-        <v>3rd PARTIES</v>
-      </c>
-      <c r="B34" s="26">
-        <f t="shared" ref="B34" si="1">SUM(B36:B48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="str">
+        <v>Consell De Cent 222</v>
+      </c>
+      <c r="B34" s="29">
+        <f>IF($A34&lt;&gt;"",SUMIF('data-services'!$A:$A,$A34,'data-services'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="str">
         <f>IF(Beds!A35&lt;&gt;"",Beds!A35,"")</f>
-        <v>BARCELONA</v>
-      </c>
-      <c r="B35" s="27">
-        <f t="shared" ref="B35" si="2">SUM(B36:B43)</f>
+        <v>Còrsega 52</v>
+      </c>
+      <c r="B35" s="29">
+        <f>IF($A35&lt;&gt;"",SUMIF('data-services'!$A:$A,$A35,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="str">
+      <c r="A36" s="13" t="str">
         <f>IF(Beds!A36&lt;&gt;"",Beds!A36,"")</f>
-        <v>Artesania 30</v>
-      </c>
-      <c r="B36" s="28">
-        <f>IF($A36&lt;&gt;"",SUMIF('data-services'!$A:$A,$A36,'data-services'!E:E),"")</f>
+        <v>Còrsega 207</v>
+      </c>
+      <c r="B36" s="29">
+        <f>IF($A36&lt;&gt;"",SUMIF('data-services'!$A:$A,$A36,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f>IF(Beds!A37&lt;&gt;"",Beds!A37,"")</f>
-        <v>Bailén 33</v>
+        <v>Encarnación 160</v>
       </c>
       <c r="B37" s="29">
-        <f>IF($A37&lt;&gt;"",SUMIF('data-services'!$A:$A,$A37,'data-services'!E:E),"")</f>
+        <f>IF($A37&lt;&gt;"",SUMIF('data-services'!$A:$A,$A37,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f>IF(Beds!A38&lt;&gt;"",Beds!A38,"")</f>
-        <v>Consell De Cent 222</v>
+        <v>Gran Via 598</v>
       </c>
       <c r="B38" s="29">
-        <f>IF($A38&lt;&gt;"",SUMIF('data-services'!$A:$A,$A38,'data-services'!E:E),"")</f>
+        <f>IF($A38&lt;&gt;"",SUMIF('data-services'!$A:$A,$A38,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f>IF(Beds!A39&lt;&gt;"",Beds!A39,"")</f>
-        <v>Còrsega 52</v>
+        <v>Ramón Albó 6</v>
       </c>
       <c r="B39" s="29">
-        <f>IF($A39&lt;&gt;"",SUMIF('data-services'!$A:$A,$A39,'data-services'!E:E),"")</f>
+        <f>IF($A39&lt;&gt;"",SUMIF('data-services'!$A:$A,$A39,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f>IF(Beds!A40&lt;&gt;"",Beds!A40,"")</f>
-        <v>Còrsega 207</v>
+        <v>Robrenyo 67</v>
       </c>
       <c r="B40" s="29">
-        <f>IF($A40&lt;&gt;"",SUMIF('data-services'!$A:$A,$A40,'data-services'!E:E),"")</f>
+        <f>IF($A40&lt;&gt;"",SUMIF('data-services'!$A:$A,$A40,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f>IF(Beds!A41&lt;&gt;"",Beds!A41,"")</f>
-        <v>Encarnación 160</v>
+        <v>Sardenya 326</v>
       </c>
       <c r="B41" s="29">
-        <f>IF($A41&lt;&gt;"",SUMIF('data-services'!$A:$A,$A41,'data-services'!E:E),"")</f>
+        <f>IF($A41&lt;&gt;"",SUMIF('data-services'!$A:$A,$A41,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f>IF(Beds!A42&lt;&gt;"",Beds!A42,"")</f>
-        <v>Gran Via 598</v>
+        <v>Travessera 43</v>
       </c>
       <c r="B42" s="29">
-        <f>IF($A42&lt;&gt;"",SUMIF('data-services'!$A:$A,$A42,'data-services'!E:E),"")</f>
+        <f>IF($A42&lt;&gt;"",SUMIF('data-services'!$A:$A,$A42,'data-services'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="str">
+      <c r="A43" s="16" t="str">
         <f>IF(Beds!A43&lt;&gt;"",Beds!A43,"")</f>
-        <v>Ramón Albó 6</v>
-      </c>
-      <c r="B43" s="29">
-        <f>IF($A43&lt;&gt;"",SUMIF('data-services'!$A:$A,$A43,'data-services'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="str">
-        <f>IF(Beds!A44&lt;&gt;"",Beds!A44,"")</f>
-        <v>Robrenyo 67</v>
-      </c>
-      <c r="B44" s="29">
-        <f>IF($A44&lt;&gt;"",SUMIF('data-services'!$A:$A,$A44,'data-services'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="str">
-        <f>IF(Beds!A45&lt;&gt;"",Beds!A45,"")</f>
-        <v>Sardenya 326</v>
-      </c>
-      <c r="B45" s="29">
-        <f>IF($A45&lt;&gt;"",SUMIF('data-services'!$A:$A,$A45,'data-services'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="str">
-        <f>IF(Beds!A46&lt;&gt;"",Beds!A46,"")</f>
-        <v>Travessera 43</v>
-      </c>
-      <c r="B46" s="29">
-        <f>IF($A46&lt;&gt;"",SUMIF('data-services'!$A:$A,$A46,'data-services'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="str">
-        <f>IF(Beds!A48&lt;&gt;"",Beds!A48,"")</f>
-        <v/>
-      </c>
-      <c r="B48" s="31" t="str">
-        <f>IF($A48&lt;&gt;"",SUMIF('data-services'!$A:$A,$A48,'data-services'!E:E),"")</f>
+        <v/>
+      </c>
+      <c r="B43" s="31" t="str">
+        <f>IF($A43&lt;&gt;"",SUMIF('data-services'!$A:$A,$A43,'data-services'!C:C),"")</f>
         <v/>
       </c>
     </row>
@@ -3313,7 +3218,7 @@
   <sheetPr>
     <tabColor rgb="FF08BDBD"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -3463,41 +3368,41 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="15" t="str">
         <f>IF(Beds!A16&lt;&gt;"",Beds!A16,"")</f>
         <v/>
       </c>
-      <c r="B16" s="30" t="str">
-        <f>IF($A16&lt;&gt;"",IF(Beds!B16*Occupancy!B17&lt;&gt;0,'Income rent'!B17/(Beds!B16*Occupancy!B17),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+      <c r="B16" s="31" t="str">
+        <f>IF($A16&lt;&gt;"",IF(Beds!B16*Occupancy!B16&lt;&gt;0,'Income rent'!B16/(Beds!B16*Occupancy!B16),0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="str">
         <f>IF(Beds!A17&lt;&gt;"",Beds!A17,"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="31" t="str">
+        <v>VALENCIA</v>
+      </c>
+      <c r="B17" s="27">
         <f>IF($A17&lt;&gt;"",IF(Beds!B17*Occupancy!B17&lt;&gt;0,'Income rent'!B17/(Beds!B17*Occupancy!B17),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
         <f>IF(Beds!A18&lt;&gt;"",Beds!A18,"")</f>
-        <v>VALENCIA</v>
-      </c>
-      <c r="B18" s="27">
+        <v>Rodriguez De Cepeda 044</v>
+      </c>
+      <c r="B18" s="28">
         <f>IF($A18&lt;&gt;"",IF(Beds!B18*Occupancy!B18&lt;&gt;0,'Income rent'!B18/(Beds!B18*Occupancy!B18),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="str">
+      <c r="A19" s="13" t="str">
         <f>IF(Beds!A19&lt;&gt;"",Beds!A19,"")</f>
-        <v>Rodriguez De Cepeda 044</v>
-      </c>
-      <c r="B19" s="28">
+        <v>Salamanca 46</v>
+      </c>
+      <c r="B19" s="29">
         <f>IF($A19&lt;&gt;"",IF(Beds!B19*Occupancy!B19&lt;&gt;0,'Income rent'!B19/(Beds!B19*Occupancy!B19),0),"")</f>
         <v>0</v>
       </c>
@@ -3505,169 +3410,169 @@
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="str">
         <f>IF(Beds!A20&lt;&gt;"",Beds!A20,"")</f>
-        <v>Salamanca 46</v>
+        <v>Nau 14</v>
       </c>
       <c r="B20" s="29">
-        <f>IF($A20&lt;&gt;"",IF(Beds!B20*Occupancy!B20&lt;&gt;0,'Income rent'!B20/(Beds!B20*Occupancy!B20),0),"")</f>
+        <f>IF($A20&lt;&gt;"",IF(Beds!B20*Occupancy!B19&lt;&gt;0,'Income rent'!B19/(Beds!B20*Occupancy!B19),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="str">
         <f>IF(Beds!A21&lt;&gt;"",Beds!A21,"")</f>
-        <v>Nau 14</v>
+        <v>Facultades</v>
       </c>
       <c r="B21" s="29">
-        <f>IF($A21&lt;&gt;"",IF(Beds!B21*Occupancy!B20&lt;&gt;0,'Income rent'!B20/(Beds!B21*Occupancy!B20),0),"")</f>
+        <f>IF($A21&lt;&gt;"",IF(Beds!B21*Occupancy!B21&lt;&gt;0,'Income rent'!B21/(Beds!B21*Occupancy!B21),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="15" t="str">
         <f>IF(Beds!A22&lt;&gt;"",Beds!A22,"")</f>
-        <v>Facultades</v>
-      </c>
-      <c r="B22" s="29">
+        <v/>
+      </c>
+      <c r="B22" s="31" t="str">
         <f>IF($A22&lt;&gt;"",IF(Beds!B22*Occupancy!B22&lt;&gt;0,'Income rent'!B22/(Beds!B22*Occupancy!B22),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="str">
         <f>IF(Beds!A23&lt;&gt;"",Beds!A23,"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="29" t="str">
+        <v>MADRID</v>
+      </c>
+      <c r="B23" s="27">
         <f>IF($A23&lt;&gt;"",IF(Beds!B23*Occupancy!B23&lt;&gt;0,'Income rent'!B23/(Beds!B23*Occupancy!B23),0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="str">
+      <c r="A24" s="12" t="str">
         <f>IF(Beds!A24&lt;&gt;"",Beds!A24,"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="31" t="str">
+        <v>Carlos III Campus Getafe</v>
+      </c>
+      <c r="B24" s="28">
         <f>IF($A24&lt;&gt;"",IF(Beds!B24*Occupancy!B24&lt;&gt;0,'Income rent'!B24/(Beds!B24*Occupancy!B24),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
         <f>IF(Beds!A25&lt;&gt;"",Beds!A25,"")</f>
+        <v>Donoso Cortés 75</v>
+      </c>
+      <c r="B25" s="29">
+        <f>IF($A25&lt;&gt;"",IF(Beds!B25*Occupancy!B24&lt;&gt;0,'Income rent'!B24/(Beds!B25*Occupancy!B24),0),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="str">
+        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+        <v/>
+      </c>
+      <c r="B26" s="31" t="str">
+        <f>IF($A26&lt;&gt;"",IF(Beds!B26*Occupancy!B26&lt;&gt;0,'Income rent'!B26/(Beds!B26*Occupancy!B26),0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="str">
+        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
         <v>BILBAO</v>
       </c>
-      <c r="B25" s="27">
-        <f>IF($A25&lt;&gt;"",IF(Beds!B25*Occupancy!B25&lt;&gt;0,'Income rent'!B25/(Beds!B25*Occupancy!B25),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
-        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+      <c r="B27" s="27">
+        <f>IF($A27&lt;&gt;"",IF(Beds!B27*Occupancy!B27&lt;&gt;0,'Income rent'!B27/(Beds!B27*Occupancy!B27),0),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="str">
+        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
         <v>General Concha 24</v>
       </c>
-      <c r="B26" s="28">
-        <f>IF($A26&lt;&gt;"",IF(Beds!B26*Occupancy!B26&lt;&gt;0,'Income rent'!B26/(Beds!B26*Occupancy!B26),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
-        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
-        <v/>
-      </c>
-      <c r="B27" s="29" t="str">
-        <f>IF($A27&lt;&gt;"",IF(Beds!B27*Occupancy!B27&lt;&gt;0,'Income rent'!B27/(Beds!B27*Occupancy!B27),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="str">
-        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
-        <v/>
-      </c>
-      <c r="B28" s="31" t="str">
+      <c r="B28" s="28">
         <f>IF($A28&lt;&gt;"",IF(Beds!B28*Occupancy!B28&lt;&gt;0,'Income rent'!B28/(Beds!B28*Occupancy!B28),0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="str">
         <f>IF(Beds!A29&lt;&gt;"",Beds!A29,"")</f>
-        <v>MADRID</v>
-      </c>
-      <c r="B29" s="27">
+        <v/>
+      </c>
+      <c r="B29" s="31" t="str">
         <f>IF($A29&lt;&gt;"",IF(Beds!B29*Occupancy!B29&lt;&gt;0,'Income rent'!B29/(Beds!B29*Occupancy!B29),0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="str">
+      <c r="A30" s="4" t="str">
         <f>IF(Beds!A30&lt;&gt;"",Beds!A30,"")</f>
-        <v>Carlos III Campus Getafe</v>
-      </c>
-      <c r="B30" s="28">
+        <v>3rd PARTIES</v>
+      </c>
+      <c r="B30" s="26">
         <f>IF($A30&lt;&gt;"",IF(Beds!B30*Occupancy!B30&lt;&gt;0,'Income rent'!B30/(Beds!B30*Occupancy!B30),0),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="str">
         <f>IF(Beds!A31&lt;&gt;"",Beds!A31,"")</f>
-        <v>Donoso Cortés 75</v>
-      </c>
-      <c r="B31" s="29">
-        <f>IF($A31&lt;&gt;"",IF(Beds!B31*Occupancy!B30&lt;&gt;0,'Income rent'!B30/(Beds!B31*Occupancy!B30),0),"")</f>
+        <v>BARCELONA</v>
+      </c>
+      <c r="B31" s="27">
+        <f>IF($A31&lt;&gt;"",IF(Beds!B31*Occupancy!B32&lt;&gt;0,'Income rent'!B32/(Beds!B31*Occupancy!B32),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="12" t="str">
         <f>IF(Beds!A32&lt;&gt;"",Beds!A32,"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="29" t="str">
+        <v>Artesania 30</v>
+      </c>
+      <c r="B32" s="28">
         <f>IF($A32&lt;&gt;"",IF(Beds!B32*Occupancy!B32&lt;&gt;0,'Income rent'!B32/(Beds!B32*Occupancy!B32),0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="str">
+      <c r="A33" s="13" t="str">
         <f>IF(Beds!A33&lt;&gt;"",Beds!A33,"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="31" t="str">
+        <v>Bailén 33</v>
+      </c>
+      <c r="B33" s="29">
         <f>IF($A33&lt;&gt;"",IF(Beds!B33*Occupancy!B33&lt;&gt;0,'Income rent'!B33/(Beds!B33*Occupancy!B33),0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="str">
+      <c r="A34" s="13" t="str">
         <f>IF(Beds!A34&lt;&gt;"",Beds!A34,"")</f>
-        <v>3rd PARTIES</v>
-      </c>
-      <c r="B34" s="26">
+        <v>Consell De Cent 222</v>
+      </c>
+      <c r="B34" s="29">
         <f>IF($A34&lt;&gt;"",IF(Beds!B34*Occupancy!B34&lt;&gt;0,'Income rent'!B34/(Beds!B34*Occupancy!B34),0),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="str">
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="str">
         <f>IF(Beds!A35&lt;&gt;"",Beds!A35,"")</f>
-        <v>BARCELONA</v>
-      </c>
-      <c r="B35" s="27">
-        <f>IF($A35&lt;&gt;"",IF(Beds!B35*Occupancy!B36&lt;&gt;0,'Income rent'!B36/(Beds!B35*Occupancy!B36),0),"")</f>
+        <v>Còrsega 52</v>
+      </c>
+      <c r="B35" s="29">
+        <f>IF($A35&lt;&gt;"",IF(Beds!B35*Occupancy!B35&lt;&gt;0,'Income rent'!B35/(Beds!B35*Occupancy!B35),0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="str">
+      <c r="A36" s="13" t="str">
         <f>IF(Beds!A36&lt;&gt;"",Beds!A36,"")</f>
-        <v>Artesania 30</v>
-      </c>
-      <c r="B36" s="28">
+        <v>Còrsega 207</v>
+      </c>
+      <c r="B36" s="29">
         <f>IF($A36&lt;&gt;"",IF(Beds!B36*Occupancy!B36&lt;&gt;0,'Income rent'!B36/(Beds!B36*Occupancy!B36),0),"")</f>
         <v>0</v>
       </c>
@@ -3675,7 +3580,7 @@
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f>IF(Beds!A37&lt;&gt;"",Beds!A37,"")</f>
-        <v>Bailén 33</v>
+        <v>Encarnación 160</v>
       </c>
       <c r="B37" s="29">
         <f>IF($A37&lt;&gt;"",IF(Beds!B37*Occupancy!B37&lt;&gt;0,'Income rent'!B37/(Beds!B37*Occupancy!B37),0),"")</f>
@@ -3685,7 +3590,7 @@
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f>IF(Beds!A38&lt;&gt;"",Beds!A38,"")</f>
-        <v>Consell De Cent 222</v>
+        <v>Gran Via 598</v>
       </c>
       <c r="B38" s="29">
         <f>IF($A38&lt;&gt;"",IF(Beds!B38*Occupancy!B38&lt;&gt;0,'Income rent'!B38/(Beds!B38*Occupancy!B38),0),"")</f>
@@ -3695,7 +3600,7 @@
     <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f>IF(Beds!A39&lt;&gt;"",Beds!A39,"")</f>
-        <v>Còrsega 52</v>
+        <v>Ramón Albó 6</v>
       </c>
       <c r="B39" s="29">
         <f>IF($A39&lt;&gt;"",IF(Beds!B39*Occupancy!B39&lt;&gt;0,'Income rent'!B39/(Beds!B39*Occupancy!B39),0),"")</f>
@@ -3705,7 +3610,7 @@
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f>IF(Beds!A40&lt;&gt;"",Beds!A40,"")</f>
-        <v>Còrsega 207</v>
+        <v>Robrenyo 67</v>
       </c>
       <c r="B40" s="29">
         <f>IF($A40&lt;&gt;"",IF(Beds!B40*Occupancy!B40&lt;&gt;0,'Income rent'!B40/(Beds!B40*Occupancy!B40),0),"")</f>
@@ -3715,7 +3620,7 @@
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f>IF(Beds!A41&lt;&gt;"",Beds!A41,"")</f>
-        <v>Encarnación 160</v>
+        <v>Sardenya 326</v>
       </c>
       <c r="B41" s="29">
         <f>IF($A41&lt;&gt;"",IF(Beds!B41*Occupancy!B41&lt;&gt;0,'Income rent'!B41/(Beds!B41*Occupancy!B41),0),"")</f>
@@ -3725,7 +3630,7 @@
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f>IF(Beds!A42&lt;&gt;"",Beds!A42,"")</f>
-        <v>Gran Via 598</v>
+        <v>Travessera 43</v>
       </c>
       <c r="B42" s="29">
         <f>IF($A42&lt;&gt;"",IF(Beds!B42*Occupancy!B42&lt;&gt;0,'Income rent'!B42/(Beds!B42*Occupancy!B42),0),"")</f>
@@ -3733,56 +3638,12 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="str">
+      <c r="A43" s="16" t="str">
         <f>IF(Beds!A43&lt;&gt;"",Beds!A43,"")</f>
-        <v>Ramón Albó 6</v>
-      </c>
-      <c r="B43" s="29">
+        <v/>
+      </c>
+      <c r="B43" s="31" t="str">
         <f>IF($A43&lt;&gt;"",IF(Beds!B43*Occupancy!B43&lt;&gt;0,'Income rent'!B43/(Beds!B43*Occupancy!B43),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="str">
-        <f>IF(Beds!A44&lt;&gt;"",Beds!A44,"")</f>
-        <v>Robrenyo 67</v>
-      </c>
-      <c r="B44" s="29">
-        <f>IF($A44&lt;&gt;"",IF(Beds!B44*Occupancy!B44&lt;&gt;0,'Income rent'!B44/(Beds!B44*Occupancy!B44),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="str">
-        <f>IF(Beds!A45&lt;&gt;"",Beds!A45,"")</f>
-        <v>Sardenya 326</v>
-      </c>
-      <c r="B45" s="29">
-        <f>IF($A45&lt;&gt;"",IF(Beds!B45*Occupancy!B45&lt;&gt;0,'Income rent'!B45/(Beds!B45*Occupancy!B45),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="str">
-        <f>IF(Beds!A46&lt;&gt;"",Beds!A46,"")</f>
-        <v>Travessera 43</v>
-      </c>
-      <c r="B46" s="29">
-        <f>IF($A46&lt;&gt;"",IF(Beds!B46*Occupancy!B46&lt;&gt;0,'Income rent'!B46/(Beds!B46*Occupancy!B46),0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="str">
-        <f>IF(Beds!A48&lt;&gt;"",Beds!A48,"")</f>
-        <v/>
-      </c>
-      <c r="B48" s="31" t="str">
-        <f>IF($A48&lt;&gt;"",IF(Beds!B48*Occupancy!B48&lt;&gt;0,'Income rent'!B48/(Beds!B48*Occupancy!B48),0),"")</f>
         <v/>
       </c>
     </row>
@@ -3798,7 +3659,7 @@
   <sheetPr>
     <tabColor rgb="FF08BDBD"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -3948,41 +3809,41 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="15" t="str">
         <f>IF(Beds!A16&lt;&gt;"",Beds!A16,"")</f>
         <v/>
       </c>
-      <c r="B16" s="30" t="str">
-        <f>IF($A16&lt;&gt;"",IF(Beds!B16&lt;&gt;0,'Income rent'!B17/Beds!B16,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+      <c r="B16" s="31" t="str">
+        <f>IF($A16&lt;&gt;"",IF(Beds!B16&lt;&gt;0,'Income rent'!B16/Beds!B16,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="str">
         <f>IF(Beds!A17&lt;&gt;"",Beds!A17,"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="31" t="str">
+        <v>VALENCIA</v>
+      </c>
+      <c r="B17" s="27">
         <f>IF($A17&lt;&gt;"",IF(Beds!B17&lt;&gt;0,'Income rent'!B17/Beds!B17,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
         <f>IF(Beds!A18&lt;&gt;"",Beds!A18,"")</f>
-        <v>VALENCIA</v>
-      </c>
-      <c r="B18" s="27">
+        <v>Rodriguez De Cepeda 044</v>
+      </c>
+      <c r="B18" s="28">
         <f>IF($A18&lt;&gt;"",IF(Beds!B18&lt;&gt;0,'Income rent'!B18/Beds!B18,0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="str">
+      <c r="A19" s="13" t="str">
         <f>IF(Beds!A19&lt;&gt;"",Beds!A19,"")</f>
-        <v>Rodriguez De Cepeda 044</v>
-      </c>
-      <c r="B19" s="28">
+        <v>Salamanca 46</v>
+      </c>
+      <c r="B19" s="29">
         <f>IF($A19&lt;&gt;"",IF(Beds!B19&lt;&gt;0,'Income rent'!B19/Beds!B19,0),"")</f>
         <v>0</v>
       </c>
@@ -3990,169 +3851,169 @@
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="str">
         <f>IF(Beds!A20&lt;&gt;"",Beds!A20,"")</f>
-        <v>Salamanca 46</v>
+        <v>Nau 14</v>
       </c>
       <c r="B20" s="29">
-        <f>IF($A20&lt;&gt;"",IF(Beds!B20&lt;&gt;0,'Income rent'!B20/Beds!B20,0),"")</f>
+        <f>IF($A20&lt;&gt;"",IF(Beds!B20&lt;&gt;0,'Income rent'!B19/Beds!B20,0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="str">
         <f>IF(Beds!A21&lt;&gt;"",Beds!A21,"")</f>
-        <v>Nau 14</v>
+        <v>Facultades</v>
       </c>
       <c r="B21" s="29">
-        <f>IF($A21&lt;&gt;"",IF(Beds!B21&lt;&gt;0,'Income rent'!B20/Beds!B21,0),"")</f>
+        <f>IF($A21&lt;&gt;"",IF(Beds!B21&lt;&gt;0,'Income rent'!B21/Beds!B21,0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="15" t="str">
         <f>IF(Beds!A22&lt;&gt;"",Beds!A22,"")</f>
-        <v>Facultades</v>
-      </c>
-      <c r="B22" s="29">
+        <v/>
+      </c>
+      <c r="B22" s="31" t="str">
         <f>IF($A22&lt;&gt;"",IF(Beds!B22&lt;&gt;0,'Income rent'!B22/Beds!B22,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="str">
         <f>IF(Beds!A23&lt;&gt;"",Beds!A23,"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="29" t="str">
+        <v>MADRID</v>
+      </c>
+      <c r="B23" s="27">
         <f>IF($A23&lt;&gt;"",IF(Beds!B23&lt;&gt;0,'Income rent'!B23/Beds!B23,0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="str">
+      <c r="A24" s="12" t="str">
         <f>IF(Beds!A24&lt;&gt;"",Beds!A24,"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="31" t="str">
+        <v>Carlos III Campus Getafe</v>
+      </c>
+      <c r="B24" s="28">
         <f>IF($A24&lt;&gt;"",IF(Beds!B24&lt;&gt;0,'Income rent'!B24/Beds!B24,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
         <f>IF(Beds!A25&lt;&gt;"",Beds!A25,"")</f>
+        <v>Donoso Cortés 75</v>
+      </c>
+      <c r="B25" s="29">
+        <f>IF($A25&lt;&gt;"",IF(Beds!B25&lt;&gt;0,'Income rent'!B24/Beds!B25,0),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="str">
+        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+        <v/>
+      </c>
+      <c r="B26" s="31" t="str">
+        <f>IF($A26&lt;&gt;"",IF(Beds!B26&lt;&gt;0,'Income rent'!B26/Beds!B26,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="str">
+        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
         <v>BILBAO</v>
       </c>
-      <c r="B25" s="27">
-        <f>IF($A25&lt;&gt;"",IF(Beds!B25&lt;&gt;0,'Income rent'!B25/Beds!B25,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
-        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+      <c r="B27" s="27">
+        <f>IF($A27&lt;&gt;"",IF(Beds!B27&lt;&gt;0,'Income rent'!B27/Beds!B27,0),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="str">
+        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
         <v>General Concha 24</v>
       </c>
-      <c r="B26" s="28">
-        <f>IF($A26&lt;&gt;"",IF(Beds!B26&lt;&gt;0,'Income rent'!B26/Beds!B26,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
-        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
-        <v/>
-      </c>
-      <c r="B27" s="29" t="str">
-        <f>IF($A27&lt;&gt;"",IF(Beds!B27&lt;&gt;0,'Income rent'!B27/Beds!B27,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="str">
-        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
-        <v/>
-      </c>
-      <c r="B28" s="31" t="str">
+      <c r="B28" s="28">
         <f>IF($A28&lt;&gt;"",IF(Beds!B28&lt;&gt;0,'Income rent'!B28/Beds!B28,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="str">
         <f>IF(Beds!A29&lt;&gt;"",Beds!A29,"")</f>
-        <v>MADRID</v>
-      </c>
-      <c r="B29" s="27">
+        <v/>
+      </c>
+      <c r="B29" s="31" t="str">
         <f>IF($A29&lt;&gt;"",IF(Beds!B29&lt;&gt;0,'Income rent'!B29/Beds!B29,0),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="str">
+      <c r="A30" s="4" t="str">
         <f>IF(Beds!A30&lt;&gt;"",Beds!A30,"")</f>
-        <v>Carlos III Campus Getafe</v>
-      </c>
-      <c r="B30" s="28">
+        <v>3rd PARTIES</v>
+      </c>
+      <c r="B30" s="26">
         <f>IF($A30&lt;&gt;"",IF(Beds!B30&lt;&gt;0,'Income rent'!B30/Beds!B30,0),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="str">
         <f>IF(Beds!A31&lt;&gt;"",Beds!A31,"")</f>
-        <v>Donoso Cortés 75</v>
-      </c>
-      <c r="B31" s="29">
-        <f>IF($A31&lt;&gt;"",IF(Beds!B31&lt;&gt;0,'Income rent'!B30/Beds!B31,0),"")</f>
+        <v>BARCELONA</v>
+      </c>
+      <c r="B31" s="27">
+        <f>IF($A31&lt;&gt;"",IF(Beds!B31&lt;&gt;0,'Income rent'!B32/Beds!B31,0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="12" t="str">
         <f>IF(Beds!A32&lt;&gt;"",Beds!A32,"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="29" t="str">
+        <v>Artesania 30</v>
+      </c>
+      <c r="B32" s="28">
         <f>IF($A32&lt;&gt;"",IF(Beds!B32&lt;&gt;0,'Income rent'!B32/Beds!B32,0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="str">
+      <c r="A33" s="13" t="str">
         <f>IF(Beds!A33&lt;&gt;"",Beds!A33,"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="31" t="str">
+        <v>Bailén 33</v>
+      </c>
+      <c r="B33" s="29">
         <f>IF($A33&lt;&gt;"",IF(Beds!B33&lt;&gt;0,'Income rent'!B33/Beds!B33,0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="str">
+      <c r="A34" s="13" t="str">
         <f>IF(Beds!A34&lt;&gt;"",Beds!A34,"")</f>
-        <v>3rd PARTIES</v>
-      </c>
-      <c r="B34" s="26">
+        <v>Consell De Cent 222</v>
+      </c>
+      <c r="B34" s="29">
         <f>IF($A34&lt;&gt;"",IF(Beds!B34&lt;&gt;0,'Income rent'!B34/Beds!B34,0),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="str">
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="str">
         <f>IF(Beds!A35&lt;&gt;"",Beds!A35,"")</f>
-        <v>BARCELONA</v>
-      </c>
-      <c r="B35" s="27">
-        <f>IF($A35&lt;&gt;"",IF(Beds!B35&lt;&gt;0,'Income rent'!B36/Beds!B35,0),"")</f>
+        <v>Còrsega 52</v>
+      </c>
+      <c r="B35" s="29">
+        <f>IF($A35&lt;&gt;"",IF(Beds!B35&lt;&gt;0,'Income rent'!B35/Beds!B35,0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="str">
+      <c r="A36" s="13" t="str">
         <f>IF(Beds!A36&lt;&gt;"",Beds!A36,"")</f>
-        <v>Artesania 30</v>
-      </c>
-      <c r="B36" s="28">
+        <v>Còrsega 207</v>
+      </c>
+      <c r="B36" s="29">
         <f>IF($A36&lt;&gt;"",IF(Beds!B36&lt;&gt;0,'Income rent'!B36/Beds!B36,0),"")</f>
         <v>0</v>
       </c>
@@ -4160,7 +4021,7 @@
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f>IF(Beds!A37&lt;&gt;"",Beds!A37,"")</f>
-        <v>Bailén 33</v>
+        <v>Encarnación 160</v>
       </c>
       <c r="B37" s="29">
         <f>IF($A37&lt;&gt;"",IF(Beds!B37&lt;&gt;0,'Income rent'!B37/Beds!B37,0),"")</f>
@@ -4170,7 +4031,7 @@
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f>IF(Beds!A38&lt;&gt;"",Beds!A38,"")</f>
-        <v>Consell De Cent 222</v>
+        <v>Gran Via 598</v>
       </c>
       <c r="B38" s="29">
         <f>IF($A38&lt;&gt;"",IF(Beds!B38&lt;&gt;0,'Income rent'!B38/Beds!B38,0),"")</f>
@@ -4180,7 +4041,7 @@
     <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f>IF(Beds!A39&lt;&gt;"",Beds!A39,"")</f>
-        <v>Còrsega 52</v>
+        <v>Ramón Albó 6</v>
       </c>
       <c r="B39" s="29">
         <f>IF($A39&lt;&gt;"",IF(Beds!B39&lt;&gt;0,'Income rent'!B39/Beds!B39,0),"")</f>
@@ -4190,7 +4051,7 @@
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f>IF(Beds!A40&lt;&gt;"",Beds!A40,"")</f>
-        <v>Còrsega 207</v>
+        <v>Robrenyo 67</v>
       </c>
       <c r="B40" s="29">
         <f>IF($A40&lt;&gt;"",IF(Beds!B40&lt;&gt;0,'Income rent'!B40/Beds!B40,0),"")</f>
@@ -4200,7 +4061,7 @@
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f>IF(Beds!A41&lt;&gt;"",Beds!A41,"")</f>
-        <v>Encarnación 160</v>
+        <v>Sardenya 326</v>
       </c>
       <c r="B41" s="29">
         <f>IF($A41&lt;&gt;"",IF(Beds!B41&lt;&gt;0,'Income rent'!B41/Beds!B41,0),"")</f>
@@ -4210,7 +4071,7 @@
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f>IF(Beds!A42&lt;&gt;"",Beds!A42,"")</f>
-        <v>Gran Via 598</v>
+        <v>Travessera 43</v>
       </c>
       <c r="B42" s="29">
         <f>IF($A42&lt;&gt;"",IF(Beds!B42&lt;&gt;0,'Income rent'!B42/Beds!B42,0),"")</f>
@@ -4218,56 +4079,12 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="str">
+      <c r="A43" s="16" t="str">
         <f>IF(Beds!A43&lt;&gt;"",Beds!A43,"")</f>
-        <v>Ramón Albó 6</v>
-      </c>
-      <c r="B43" s="29">
+        <v/>
+      </c>
+      <c r="B43" s="31" t="str">
         <f>IF($A43&lt;&gt;"",IF(Beds!B43&lt;&gt;0,'Income rent'!B43/Beds!B43,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="str">
-        <f>IF(Beds!A44&lt;&gt;"",Beds!A44,"")</f>
-        <v>Robrenyo 67</v>
-      </c>
-      <c r="B44" s="29">
-        <f>IF($A44&lt;&gt;"",IF(Beds!B44&lt;&gt;0,'Income rent'!B44/Beds!B44,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="str">
-        <f>IF(Beds!A45&lt;&gt;"",Beds!A45,"")</f>
-        <v>Sardenya 326</v>
-      </c>
-      <c r="B45" s="29">
-        <f>IF($A45&lt;&gt;"",IF(Beds!B45&lt;&gt;0,'Income rent'!B45/Beds!B45,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="str">
-        <f>IF(Beds!A46&lt;&gt;"",Beds!A46,"")</f>
-        <v>Travessera 43</v>
-      </c>
-      <c r="B46" s="29">
-        <f>IF($A46&lt;&gt;"",IF(Beds!B46&lt;&gt;0,'Income rent'!B46/Beds!B46,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="str">
-        <f>IF(Beds!A48&lt;&gt;"",Beds!A48,"")</f>
-        <v/>
-      </c>
-      <c r="B48" s="31" t="str">
-        <f>IF($A48&lt;&gt;"",IF(Beds!B48&lt;&gt;0,'Income rent'!B48/Beds!B48,0),"")</f>
         <v/>
       </c>
     </row>
@@ -4283,7 +4100,7 @@
   <sheetPr>
     <tabColor rgb="FF08BDBD"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -4318,7 +4135,7 @@
         <v>TOTAL</v>
       </c>
       <c r="B4" s="39">
-        <f>B5+B34</f>
+        <f>B5+B30</f>
         <v>0</v>
       </c>
     </row>
@@ -4328,7 +4145,7 @@
         <v>VANDOR</v>
       </c>
       <c r="B5" s="40">
-        <f>B6+B18+B25+B29</f>
+        <f>B6+B17+B27+B23</f>
         <v>0</v>
       </c>
     </row>
@@ -4338,7 +4155,7 @@
         <v>BARCELONA</v>
       </c>
       <c r="B6" s="41">
-        <f>SUM(B7:B17)</f>
+        <f>SUM(B7:B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -4348,7 +4165,7 @@
         <v>Balmes 335</v>
       </c>
       <c r="B7" s="42">
-        <f>IF($A7&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A7,'data-nights'!E:E),"")</f>
+        <f>IF($A7&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A7,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4358,7 +4175,7 @@
         <v>Nàpols 206</v>
       </c>
       <c r="B8" s="43">
-        <f>IF($A8&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A8,'data-nights'!E:E),"")</f>
+        <f>IF($A8&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A8,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4368,7 +4185,7 @@
         <v>Rocafort 219</v>
       </c>
       <c r="B9" s="43">
-        <f>IF($A9&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A9,'data-nights'!E:E),"")</f>
+        <f>IF($A9&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A9,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4378,7 +4195,7 @@
         <v>Entença 069</v>
       </c>
       <c r="B10" s="43">
-        <f>IF($A10&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A10,'data-nights'!E:E),"")</f>
+        <f>IF($A10&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A10,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4388,7 +4205,7 @@
         <v>Avenida Madrid 110</v>
       </c>
       <c r="B11" s="43">
-        <f>IF($A11&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A11,'data-nights'!E:E),"")</f>
+        <f>IF($A11&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A11,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4398,7 +4215,7 @@
         <v>Muntaner 448</v>
       </c>
       <c r="B12" s="43">
-        <f>IF($A12&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A12,'data-nights'!E:E),"")</f>
+        <f>IF($A12&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A12,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4408,7 +4225,7 @@
         <v>Concordia 12</v>
       </c>
       <c r="B13" s="43">
-        <f>IF($A13&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A13,'data-nights'!E:E),"")</f>
+        <f>IF($A13&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A13,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4418,7 +4235,7 @@
         <v>Consell De Cent 538</v>
       </c>
       <c r="B14" s="43">
-        <f>IF($A14&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A14,'data-nights'!E:E),"")</f>
+        <f>IF($A14&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A14,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -4428,331 +4245,287 @@
         <v>Còrsega 396</v>
       </c>
       <c r="B15" s="44">
-        <f>IF($A15&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A15,'data-nights'!E:E),"")</f>
+        <f>IF($A15&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A15,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="15" t="str">
         <f>IF(Beds!A16&lt;&gt;"",Beds!A16,"")</f>
         <v/>
       </c>
-      <c r="B16" s="44" t="str">
-        <f>IF($A16&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A16,'data-nights'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+      <c r="B16" s="45" t="str">
+        <f>IF($A16&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A16,'data-nights'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="str">
         <f>IF(Beds!A17&lt;&gt;"",Beds!A17,"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="45" t="str">
-        <f>IF($A17&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A17,'data-nights'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
+        <v>VALENCIA</v>
+      </c>
+      <c r="B17" s="41">
+        <f>SUM(B18:B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
         <f>IF(Beds!A18&lt;&gt;"",Beds!A18,"")</f>
-        <v>VALENCIA</v>
-      </c>
-      <c r="B18" s="41">
-        <f>SUM(B19:B24)</f>
+        <v>Rodriguez De Cepeda 044</v>
+      </c>
+      <c r="B18" s="42">
+        <f>IF($A18&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A18,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="str">
+      <c r="A19" s="13" t="str">
         <f>IF(Beds!A19&lt;&gt;"",Beds!A19,"")</f>
-        <v>Rodriguez De Cepeda 044</v>
-      </c>
-      <c r="B19" s="42">
-        <f>IF($A19&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A19,'data-nights'!E:E),"")</f>
+        <v>Salamanca 46</v>
+      </c>
+      <c r="B19" s="43">
+        <f>IF($A19&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A19,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="str">
         <f>IF(Beds!A20&lt;&gt;"",Beds!A20,"")</f>
-        <v>Salamanca 46</v>
+        <v>Nau 14</v>
       </c>
       <c r="B20" s="43">
-        <f>IF($A20&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A20,'data-nights'!E:E),"")</f>
+        <f>IF($A20&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A20,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="str">
         <f>IF(Beds!A21&lt;&gt;"",Beds!A21,"")</f>
-        <v>Nau 14</v>
+        <v>Facultades</v>
       </c>
       <c r="B21" s="43">
-        <f>IF($A21&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A21,'data-nights'!E:E),"")</f>
+        <f>IF($A21&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A21,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="15" t="str">
         <f>IF(Beds!A22&lt;&gt;"",Beds!A22,"")</f>
-        <v>Facultades</v>
-      </c>
-      <c r="B22" s="43">
-        <f>IF($A22&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A22,'data-nights'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
+        <v/>
+      </c>
+      <c r="B22" s="45" t="str">
+        <f>IF($A22&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A22,'data-nights'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="str">
         <f>IF(Beds!A23&lt;&gt;"",Beds!A23,"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="43" t="str">
-        <f>IF($A23&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A23,'data-nights'!E:E),"")</f>
-        <v/>
+        <v>MADRID</v>
+      </c>
+      <c r="B23" s="41">
+        <f>SUM(B24:B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="str">
+      <c r="A24" s="12" t="str">
         <f>IF(Beds!A24&lt;&gt;"",Beds!A24,"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="45" t="str">
-        <f>IF($A24&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A24,'data-nights'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="str">
+        <v>Carlos III Campus Getafe</v>
+      </c>
+      <c r="B24" s="42">
+        <f>IF($A24&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A24,'data-nights'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
         <f>IF(Beds!A25&lt;&gt;"",Beds!A25,"")</f>
+        <v>Donoso Cortés 75</v>
+      </c>
+      <c r="B25" s="43">
+        <f>IF($A25&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A25,'data-nights'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="str">
+        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+        <v/>
+      </c>
+      <c r="B26" s="45" t="str">
+        <f>IF($A26&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A26,'data-nights'!C:C),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="str">
+        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
         <v>BILBAO</v>
       </c>
-      <c r="B25" s="41">
-        <f>SUM(B26:B28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
-        <f>IF(Beds!A26&lt;&gt;"",Beds!A26,"")</f>
+      <c r="B27" s="41">
+        <f>SUM(B28:B29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="str">
+        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
         <v>General Concha 24</v>
       </c>
-      <c r="B26" s="42">
-        <f>IF($A26&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A26,'data-nights'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
-        <f>IF(Beds!A27&lt;&gt;"",Beds!A27,"")</f>
-        <v/>
-      </c>
-      <c r="B27" s="43" t="str">
-        <f>IF($A27&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A27,'data-nights'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="str">
-        <f>IF(Beds!A28&lt;&gt;"",Beds!A28,"")</f>
-        <v/>
-      </c>
-      <c r="B28" s="45" t="str">
-        <f>IF($A28&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A28,'data-nights'!E:E),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="str">
+      <c r="B28" s="42">
+        <f>IF($A28&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A28,'data-nights'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="str">
         <f>IF(Beds!A29&lt;&gt;"",Beds!A29,"")</f>
-        <v>MADRID</v>
-      </c>
-      <c r="B29" s="41">
-        <f>SUM(B30:B33)</f>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="B29" s="45" t="str">
+        <f>IF($A29&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A29,'data-nights'!C:C),"")</f>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="str">
+      <c r="A30" s="4" t="str">
         <f>IF(Beds!A30&lt;&gt;"",Beds!A30,"")</f>
-        <v>Carlos III Campus Getafe</v>
-      </c>
-      <c r="B30" s="42">
-        <f>IF($A30&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A30,'data-nights'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+        <v>3rd PARTIES</v>
+      </c>
+      <c r="B30" s="40">
+        <f>SUM(B32:B43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="str">
         <f>IF(Beds!A31&lt;&gt;"",Beds!A31,"")</f>
-        <v>Donoso Cortés 75</v>
-      </c>
-      <c r="B31" s="43">
-        <f>IF($A31&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A31,'data-nights'!E:E),"")</f>
+        <v>BARCELONA</v>
+      </c>
+      <c r="B31" s="41">
+        <f t="shared" ref="B31" si="1">SUM(B32:B39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="12" t="str">
         <f>IF(Beds!A32&lt;&gt;"",Beds!A32,"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="43" t="str">
-        <f>IF($A32&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A32,'data-nights'!E:E),"")</f>
-        <v/>
+        <v>Artesania 30</v>
+      </c>
+      <c r="B32" s="42">
+        <f>IF($A32&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A32,'data-nights'!C:C),"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="str">
+      <c r="A33" s="13" t="str">
         <f>IF(Beds!A33&lt;&gt;"",Beds!A33,"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="45" t="str">
-        <f>IF($A33&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A33,'data-nights'!E:E),"")</f>
-        <v/>
+        <v>Bailén 33</v>
+      </c>
+      <c r="B33" s="43">
+        <f>IF($A33&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A33,'data-nights'!C:C),"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="str">
+      <c r="A34" s="13" t="str">
         <f>IF(Beds!A34&lt;&gt;"",Beds!A34,"")</f>
-        <v>3rd PARTIES</v>
-      </c>
-      <c r="B34" s="40">
-        <f t="shared" ref="B34" si="1">SUM(B36:B48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="str">
+        <v>Consell De Cent 222</v>
+      </c>
+      <c r="B34" s="43">
+        <f>IF($A34&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A34,'data-nights'!C:C),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="str">
         <f>IF(Beds!A35&lt;&gt;"",Beds!A35,"")</f>
-        <v>BARCELONA</v>
-      </c>
-      <c r="B35" s="41">
-        <f t="shared" ref="B35" si="2">SUM(B36:B43)</f>
+        <v>Còrsega 52</v>
+      </c>
+      <c r="B35" s="43">
+        <f>IF($A35&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A35,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="str">
+      <c r="A36" s="13" t="str">
         <f>IF(Beds!A36&lt;&gt;"",Beds!A36,"")</f>
-        <v>Artesania 30</v>
-      </c>
-      <c r="B36" s="42">
-        <f>IF($A36&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A36,'data-nights'!E:E),"")</f>
+        <v>Còrsega 207</v>
+      </c>
+      <c r="B36" s="43">
+        <f>IF($A36&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A36,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f>IF(Beds!A37&lt;&gt;"",Beds!A37,"")</f>
-        <v>Bailén 33</v>
+        <v>Encarnación 160</v>
       </c>
       <c r="B37" s="43">
-        <f>IF($A37&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A37,'data-nights'!E:E),"")</f>
+        <f>IF($A37&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A37,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f>IF(Beds!A38&lt;&gt;"",Beds!A38,"")</f>
-        <v>Consell De Cent 222</v>
+        <v>Gran Via 598</v>
       </c>
       <c r="B38" s="43">
-        <f>IF($A38&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A38,'data-nights'!E:E),"")</f>
+        <f>IF($A38&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A38,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f>IF(Beds!A39&lt;&gt;"",Beds!A39,"")</f>
-        <v>Còrsega 52</v>
+        <v>Ramón Albó 6</v>
       </c>
       <c r="B39" s="43">
-        <f>IF($A39&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A39,'data-nights'!E:E),"")</f>
+        <f>IF($A39&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A39,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f>IF(Beds!A40&lt;&gt;"",Beds!A40,"")</f>
-        <v>Còrsega 207</v>
+        <v>Robrenyo 67</v>
       </c>
       <c r="B40" s="43">
-        <f>IF($A40&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A40,'data-nights'!E:E),"")</f>
+        <f>IF($A40&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A40,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f>IF(Beds!A41&lt;&gt;"",Beds!A41,"")</f>
-        <v>Encarnación 160</v>
+        <v>Sardenya 326</v>
       </c>
       <c r="B41" s="43">
-        <f>IF($A41&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A41,'data-nights'!E:E),"")</f>
+        <f>IF($A41&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A41,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f>IF(Beds!A42&lt;&gt;"",Beds!A42,"")</f>
-        <v>Gran Via 598</v>
+        <v>Travessera 43</v>
       </c>
       <c r="B42" s="43">
-        <f>IF($A42&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A42,'data-nights'!E:E),"")</f>
+        <f>IF($A42&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A42,'data-nights'!C:C),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="str">
+      <c r="A43" s="16" t="str">
         <f>IF(Beds!A43&lt;&gt;"",Beds!A43,"")</f>
-        <v>Ramón Albó 6</v>
-      </c>
-      <c r="B43" s="43">
-        <f>IF($A43&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A43,'data-nights'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="str">
-        <f>IF(Beds!A44&lt;&gt;"",Beds!A44,"")</f>
-        <v>Robrenyo 67</v>
-      </c>
-      <c r="B44" s="43">
-        <f>IF($A44&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A44,'data-nights'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="str">
-        <f>IF(Beds!A45&lt;&gt;"",Beds!A45,"")</f>
-        <v>Sardenya 326</v>
-      </c>
-      <c r="B45" s="43">
-        <f>IF($A45&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A45,'data-nights'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="str">
-        <f>IF(Beds!A46&lt;&gt;"",Beds!A46,"")</f>
-        <v>Travessera 43</v>
-      </c>
-      <c r="B46" s="43">
-        <f>IF($A46&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A46,'data-nights'!E:E),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="44"/>
-    </row>
-    <row r="48" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="str">
-        <f>IF(Beds!A48&lt;&gt;"",Beds!A48,"")</f>
-        <v/>
-      </c>
-      <c r="B48" s="45" t="str">
-        <f>IF($A48&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A48,'data-nights'!E:E),"")</f>
+        <v/>
+      </c>
+      <c r="B43" s="45" t="str">
+        <f>IF($A43&lt;&gt;"",SUMIF('data-nights'!$A:$A,$A43,'data-nights'!C:C),"")</f>
         <v/>
       </c>
     </row>
@@ -4765,21 +4538,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:BP1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="2" width="21" customWidth="1"/>
+    <col min="3" max="68" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -4799,6 +4573,54 @@
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="10"/>
+      <c r="BD1" s="10"/>
+      <c r="BE1" s="10"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="10"/>
+      <c r="BJ1" s="10"/>
+      <c r="BK1" s="10"/>
+      <c r="BL1" s="10"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="10"/>
+      <c r="BO1" s="10"/>
+      <c r="BP1" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4807,28 +4629,25 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:BP1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="2" width="21" customWidth="1"/>
+    <col min="3" max="68" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
@@ -4843,8 +4662,50 @@
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BE1" s="10"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="10"/>
+      <c r="BJ1" s="10"/>
+      <c r="BK1" s="10"/>
+      <c r="BL1" s="10"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="10"/>
+      <c r="BO1" s="10"/>
+      <c r="BP1" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>